<commit_message>
feat: Mejora de plantillas HTML y estilos para el menú y tarjetas de oferta
</commit_message>
<xml_diff>
--- a/dist/menu_test.xlsx
+++ b/dist/menu_test.xlsx
@@ -4,7 +4,14 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Refrescos y Aguas" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Cerveza 33CL" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Vinos Blancos y Tintos" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Chupitos" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Cerveza 33CL" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Cerveza Barril" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Mojito Cubano" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Daiquiry" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Cafe e infuciones" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Postres y Helados" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>product</t>
   </si>
@@ -48,16 +55,103 @@
   </si>
   <si>
     <t>MONSTER ENERGY</t>
+  </si>
+  <si>
+    <t>rioja crianza copa</t>
+  </si>
+  <si>
+    <t>ribera del duero copa</t>
+  </si>
+  <si>
+    <t>verdejo rueda copa</t>
+  </si>
+  <si>
+    <t>chardonnay copa</t>
+  </si>
+  <si>
+    <t>rioja reserva botella</t>
+  </si>
+  <si>
+    <t>rosado navarro botella</t>
+  </si>
+  <si>
+    <t>albariño botella</t>
+  </si>
+  <si>
+    <t>lambrusco copa</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>caña (20 cl)</t>
+  </si>
+  <si>
+    <t>doble (40 cl)</t>
+  </si>
+  <si>
+    <t>jarra (50 cl)</t>
+  </si>
+  <si>
+    <t>tercio (33 cl)</t>
+  </si>
+  <si>
+    <t>café solo</t>
+  </si>
+  <si>
+    <t>café con leche</t>
+  </si>
+  <si>
+    <t>café cortado</t>
+  </si>
+  <si>
+    <t>cappuccino</t>
+  </si>
+  <si>
+    <t>té negro</t>
+  </si>
+  <si>
+    <t>manzanilla</t>
+  </si>
+  <si>
+    <t>infusión de frutas</t>
+  </si>
+  <si>
+    <t>café descafeinado</t>
+  </si>
+  <si>
+    <t>tarta de queso casera</t>
+  </si>
+  <si>
+    <t>brownie con helado</t>
+  </si>
+  <si>
+    <t>helado vainilla bola</t>
+  </si>
+  <si>
+    <t>helado chocolate bola</t>
+  </si>
+  <si>
+    <t>mousse de limón</t>
+  </si>
+  <si>
+    <t>fruta de temporada</t>
+  </si>
+  <si>
+    <t>copa de helado mixta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-C0A];[RED]\-#,##0.00\ [$€-C0A]"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
+    <numFmt numFmtId="166" formatCode="#,##0&quot;€&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00&quot;€&quot;"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -68,6 +162,15 @@
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <color rgb="FF1B1C1D"/>
+      <name val="&quot;Google Sans Text&quot;"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -100,6 +203,24 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -113,6 +234,34 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1418,6 +1567,132 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="28.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6">
+        <v>18.0</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6">
+        <v>22.0</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -2482,4 +2757,281 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9">
+        <v>5.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="10">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="10">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="10">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="10">
+        <v>4.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>